<commit_message>
Update baseline and special topics.
</commit_message>
<xml_diff>
--- a/_site/Data/ChildCareEC.xlsx
+++ b/_site/Data/ChildCareEC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C901B9-C3AF-5540-899A-C0C8350B28B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72206855-0CDD-A841-930C-2D8D26A05E32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="22020" windowHeight="15540" xr2:uid="{8A673D2B-23AC-4849-B85E-D6BED00A64B1}"/>
+    <workbookView xWindow="42460" yWindow="3840" windowWidth="27580" windowHeight="17200" xr2:uid="{8A673D2B-23AC-4849-B85E-D6BED00A64B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Question Bank " sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="96">
   <si>
     <t>Question</t>
   </si>
@@ -49,23 +49,11 @@
   </si>
   <si>
     <t>Answers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prior to the coronavirus (COVID-19) Pandemic, did you use any non-parental care for your child(ren) under the age of 5? 
-</t>
   </si>
   <si>
     <t xml:space="preserve">• Yes 
 • No 
 • Unsure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This week, have you used any non-parental care for your child(ren) under the age of 5?  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you expect your need for non-parental care for your child under the age of 5 to change in the next month?  
-</t>
   </si>
   <si>
     <t xml:space="preserve">• Yes, I will need more non-parental care 
@@ -99,15 +87,7 @@
 • At least 5 hours of paid care from a home-based child care provider. Please include home-based care where the provider is paid to care for your child even if you are not making the payment. </t>
   </si>
   <si>
-    <t xml:space="preserve">Prior to the coronavirus (COVID-19) Pandemic, how many hours on average per week was your child care for by...[based on answers above] 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">• Answer choices 1 to “more than 100 hours” </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[If cared for by a relative, friend or neighbor] What is the relationship of the relative, friend, or neighbor providing care to your child(ren) in the age range 0-5? Select all that apply.  
-</t>
   </si>
   <si>
     <t xml:space="preserve">• other parent/step parent 
@@ -148,10 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve">How many hours this week was your child cared for by... [based on answers above] 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[If cared for by a relative, friend or neighbor] What is the relationship of the relative, friend, or neighbor currently providing care to your child(ren) in the age range 0-5? Select all that apply. 
 </t>
   </si>
   <si>
@@ -194,10 +170,6 @@
 • Other, please describe: [text entry] </t>
   </si>
   <si>
-    <t xml:space="preserve">Prior to the coronavirus (COVID-19) Pandemic, how many hours on average per week was your child care for by...[based on answers above]  
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prior to the coronavirus (COVID-19) Pandemic, was the child care provided by [based on answers from above] paid or unpaid?  
 </t>
   </si>
@@ -474,22 +446,326 @@
 • Other</t>
   </si>
   <si>
-    <t xml:space="preserve">When you think about your family’s budget, if you have to pay for childcare, how much do you think is an “affordable” amount to spend on chidl care for all your children? 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">• More than 30% of your household income 
 • 20%-30% of your household income 
 • 10%-20% of your household income 
 • 5%-9% of your household income 
 • 1%-4% of your household income </t>
   </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prior to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the coronavirus (COVID-19) Pandemic, did you use any non-parental care for your child(ren) under the age of 5? 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">This week, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">have you used any non-parental care for your child(ren) under the age of 5?  
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do you expect your need for non-parental care for your child under the age of 5 to change </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in the next month</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">?  
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RAPID Team modified from the National Survey of Early Care and Education (NSECE) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developed by RAPID Team </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prior to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the coronavirus (COVID-19) Pandemic, how many hours per week on average did you utilize any type of paid or unpaid center-based care for your child(ren) in the 0-5 age range?
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prior to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the coronavirus (COVID-19) Pandemic, how many hours per week on average did you utilize any type of unpaid care by a relative, friend or neighbor for your child(ren) in the 0-5 age range?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Prior to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the coronavirus (COVID-19) Pandemic, how many hours per week on average did you utilize any type of paid care by a relative, friend or neighbor for your child(sen) in the 0-5 age range?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prior to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the coronavirus (COVID-19) Pandemic, how many hours per week on average did you utilize any type of paid care from a home-based child care provider for your child(ren) in the 0-5 age range?</t>
+    </r>
+  </si>
+  <si>
+    <t>Developed by RAPID Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the relationship of the relative, friend, or neighbor who provided  care to your child(ren) in the age range 0-5? Select all that apply.  
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Currently, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">how many hours per week on average did you utilize any type of paid or unpaid center-based care for your child(ren) in the 0-5 age range?
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Currently, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>how many hours per week on average did you utilize any type of unpaid care by a relative, friend or neighbor for your child(ren) in the 0-5 age range?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Currently, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>how many hours per week on average did you utilize any type of paid care by a relative, friend or neighbor for any child age 5 or under?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Currently,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> how many hours per week on average did you utilize any type of paid care from a home-based child care provider for your child(ren) in the 0-5 age range?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the relationship of the relative, friend, or neighbor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>currently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> providing care to your child(ren) in the age range 0-5? Select all that apply. 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">When you think about your family’s budget, if you have to pay for childcare, how much do you think is an “affordable” amount to spend on childcare for all your children? 
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -498,6 +774,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -525,11 +809,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,20 +1134,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2689D1A7-E07D-A54D-BF8D-68ACF4A3D5C5}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="75" style="3" customWidth="1"/>
+    <col min="2" max="3" width="24.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,539 +1155,689 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51">
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="102">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="238">
-      <c r="A5" s="2" t="s">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="187">
-      <c r="A6" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="51">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="20" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="372" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="372" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="102">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="187">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="238">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="102">
-      <c r="A11" s="2" t="s">
+    <row r="28" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="102">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="136">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="51">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="204">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="51">
-      <c r="A17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="51">
-      <c r="A18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="204">
-      <c r="A19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="34">
-      <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="34">
-      <c r="A21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="136">
-      <c r="A22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="238">
-      <c r="A23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="119">
-      <c r="A24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="136">
-      <c r="A25" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="68">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="68">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="119">
-      <c r="A28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="C37" s="2"/>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="85">
-      <c r="A29" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="221">
-      <c r="A30" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C39" s="2"/>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="306" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="68">
-      <c r="A31" s="2" t="s">
+      <c r="B40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="51">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="170">
-      <c r="A33" s="2" t="s">
+      <c r="C41" s="2"/>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="68">
-      <c r="A34" s="2" t="s">
+      <c r="C42" s="2"/>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="170">
-      <c r="A35" s="2" t="s">
+      <c r="C43" s="2"/>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="34">
-      <c r="A36" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C44" s="2"/>
+      <c r="D44" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="170">
-      <c r="A37" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="170">
-      <c r="A38" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C47" s="2"/>
+      <c r="D47" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="34">
-      <c r="A39" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C48" s="2"/>
+      <c r="D48" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="323" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="34">
-      <c r="A40" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="34">
-      <c r="A41" s="2" t="s">
+      <c r="C49" s="2"/>
+      <c r="D49" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="340" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="119">
-      <c r="A42" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C50" s="2"/>
+      <c r="D50" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="388" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="68">
-      <c r="A43" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C51" s="2"/>
+      <c r="D51" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="170" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="170">
-      <c r="A44" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="170">
-      <c r="A45" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="221">
-      <c r="A46" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="85">
-      <c r="A47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="34">
-      <c r="A48" s="2" t="s">
+      <c r="C52" s="2"/>
+      <c r="D52" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="51">
-      <c r="A49" s="2" t="s">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="34">
-      <c r="A50" s="2" t="s">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>